<commit_message>
[ADD]: added model results to main page
</commit_message>
<xml_diff>
--- a/models/PerformanceData/final_models_data.xlsx
+++ b/models/PerformanceData/final_models_data.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raymond Vu\Documents\GitHub\OscarPredictor\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinah/OscarPredictor/models/PerformanceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBB7DBA3-82B2-49F1-802B-340C28A1D1E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96431321-1EA1-634C-81AE-92CF031308AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="1920" windowWidth="10332" windowHeight="10788" xr2:uid="{4D8D8700-0050-4D33-84E2-A32CB3D1F920}"/>
+    <workbookView xWindow="1940" yWindow="2900" windowWidth="30920" windowHeight="14660" xr2:uid="{4D8D8700-0050-4D33-84E2-A32CB3D1F920}"/>
   </bookViews>
   <sheets>
     <sheet name="final_models_data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">final_models_data!$A$1:$E$27</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -167,10 +170,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,21 +496,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0CE4BF-8579-4BD6-98A2-FA2F6F8317A7}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -517,9 +526,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B2">
         <v>2017</v>
@@ -528,15 +537,15 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.123</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="E2">
-        <v>0.151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B3">
         <v>2017</v>
@@ -545,14 +554,14 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.14599999999999999</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="E3">
-        <v>7.5999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -568,9 +577,9 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B5">
         <v>2017</v>
@@ -579,15 +588,15 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.35399999999999998</v>
+        <v>0.115</v>
       </c>
       <c r="E5">
-        <v>0.156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
+        <v>0.159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="B6">
         <v>2017</v>
@@ -596,15 +605,15 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.28499999999999998</v>
+        <v>0.123</v>
       </c>
       <c r="E6">
-        <v>0.19500000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
+        <v>0.151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B7">
         <v>2017</v>
@@ -613,15 +622,15 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>6.9000000000000006E-2</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="E7">
-        <v>0.105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B8">
         <v>2017</v>
@@ -630,83 +639,83 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>6.9000000000000006E-2</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="E8">
-        <v>5.5E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+        <v>0.19500000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>2017</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>2017</v>
       </c>
-      <c r="C9" s="1" t="b">
+      <c r="C10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="1">
         <v>0.41499999999999998</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="1">
         <v>0.30499999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>2017</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0.115</v>
-      </c>
-      <c r="E10">
-        <v>0.159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>2018</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>2018</v>
       </c>
-      <c r="C11" s="1" t="b">
+      <c r="C12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>2018</v>
-      </c>
-      <c r="C12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="E12">
-        <v>0.13300000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B13">
         <v>2018</v>
@@ -714,16 +723,16 @@
       <c r="C13" t="b">
         <v>0</v>
       </c>
-      <c r="D13" s="1">
-        <v>0.48499999999999999</v>
+      <c r="D13">
+        <v>0.13100000000000001</v>
       </c>
       <c r="E13">
-        <v>0.17199999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>15</v>
+        <v>8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B14">
         <v>2018</v>
@@ -735,12 +744,12 @@
         <v>0.13100000000000001</v>
       </c>
       <c r="E14">
-        <v>8.8999999999999996E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B15">
         <v>2018</v>
@@ -752,12 +761,12 @@
         <v>0.23100000000000001</v>
       </c>
       <c r="E15">
-        <v>0.17699999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>17</v>
+        <v>0.13300000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B16">
         <v>2018</v>
@@ -766,15 +775,15 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0.218</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>18</v>
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="E16">
+        <v>0.17699999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B17">
         <v>2018</v>
@@ -783,15 +792,15 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="E17">
-        <v>0.185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>19</v>
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B18">
         <v>2018</v>
@@ -799,16 +808,16 @@
       <c r="C18" t="b">
         <v>0</v>
       </c>
-      <c r="D18">
-        <v>4.5999999999999999E-2</v>
+      <c r="D18" s="1">
+        <v>0.48499999999999999</v>
       </c>
       <c r="E18">
-        <v>0.10100000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>1917</v>
+        <v>0.17199999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B19">
         <v>2019</v>
@@ -817,15 +826,15 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0.308</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0.21099999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>20</v>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E19">
+        <v>8.1000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B20">
         <v>2019</v>
@@ -834,15 +843,15 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>8.5000000000000006E-2</v>
+        <v>0.108</v>
       </c>
       <c r="E20">
-        <v>8.1000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>21</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B21">
         <v>2019</v>
@@ -851,15 +860,15 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>0.123</v>
+        <v>0.115</v>
       </c>
       <c r="E21">
-        <v>6.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>22</v>
+        <v>0.16300000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B22">
         <v>2019</v>
@@ -868,32 +877,32 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>0.108</v>
+        <v>0.123</v>
       </c>
       <c r="E22">
-        <v>6.5000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
         <v>2019</v>
       </c>
-      <c r="C23" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0.438</v>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.154</v>
       </c>
       <c r="E23">
-        <v>0.20699999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>24</v>
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B24">
         <v>2019</v>
@@ -902,15 +911,15 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>0.154</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="E24">
-        <v>5.3999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>25</v>
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B25">
         <v>2019</v>
@@ -919,15 +928,15 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0.115</v>
+        <v>0.20799999999999999</v>
       </c>
       <c r="E25">
-        <v>0.16300000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>26</v>
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>1917</v>
       </c>
       <c r="B26">
         <v>2019</v>
@@ -936,30 +945,35 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="E26">
-        <v>0.105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
+        <v>0.308</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.21099999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="1">
         <v>2019</v>
       </c>
-      <c r="C27" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0.16900000000000001</v>
+      <c r="C27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.438</v>
       </c>
       <c r="E27">
-        <v>0.14299999999999999</v>
+        <v>0.20699999999999999</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E27" xr:uid="{20ED4524-3BD6-8742-B24C-87AB2F19F885}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E27">
+      <sortCondition ref="B1:B27"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added pickled model file
</commit_message>
<xml_diff>
--- a/models/PerformanceData/final_models_data.xlsx
+++ b/models/PerformanceData/final_models_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinah/OscarPredictor/models/PerformanceData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raymond Vu\Documents\GitHub\OscarPredictor\models\PerformanceData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96431321-1EA1-634C-81AE-92CF031308AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7B4E37-05EA-4205-9317-E0DA01BE86C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="2900" windowWidth="30920" windowHeight="14660" xr2:uid="{4D8D8700-0050-4D33-84E2-A32CB3D1F920}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4D8D8700-0050-4D33-84E2-A32CB3D1F920}"/>
   </bookViews>
   <sheets>
     <sheet name="final_models_data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>title</t>
   </si>
@@ -127,12 +127,42 @@
   </si>
   <si>
     <t>SVC Predictions</t>
+  </si>
+  <si>
+    <t>Arrival</t>
+  </si>
+  <si>
+    <t>Fences</t>
+  </si>
+  <si>
+    <t>Hacksaw Ridge</t>
+  </si>
+  <si>
+    <t>Hell or High Water</t>
+  </si>
+  <si>
+    <t>Hidden Figures</t>
+  </si>
+  <si>
+    <t>La La Land</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t>Manchester by the Sea</t>
+  </si>
+  <si>
+    <t>Moonlight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -173,13 +203,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,23 +522,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0CE4BF-8579-4BD6-98A2-FA2F6F8317A7}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="1" max="1" width="35" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="5.77734375" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -526,446 +554,572 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
       </c>
       <c r="B2">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>6.9000000000000006E-2</v>
+      <c r="D2" s="3">
+        <v>0.37</v>
       </c>
       <c r="E2">
         <v>0.105</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
       </c>
       <c r="B3">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
-      <c r="D3">
-        <v>6.9000000000000006E-2</v>
+      <c r="D3" s="3">
+        <v>0.13800000000000001</v>
       </c>
       <c r="E3">
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>32</v>
       </c>
       <c r="B4">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>8.5000000000000006E-2</v>
+      <c r="D4" s="3">
+        <v>0.33600000000000002</v>
       </c>
       <c r="E4">
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
       </c>
       <c r="B5">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
       </c>
-      <c r="D5">
-        <v>0.115</v>
+      <c r="D5" s="3">
+        <v>0.155</v>
       </c>
       <c r="E5">
         <v>0.159</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
       </c>
       <c r="B6">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
       </c>
-      <c r="D6">
-        <v>0.123</v>
+      <c r="D6" s="3">
+        <v>0.36</v>
       </c>
       <c r="E6">
         <v>0.151</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B7">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
-      <c r="D7">
-        <v>0.14599999999999999</v>
+      <c r="D7" s="4">
+        <v>0.39600000000000002</v>
       </c>
       <c r="E7">
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>36</v>
       </c>
       <c r="B8">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
       </c>
-      <c r="D8">
-        <v>0.28499999999999998</v>
+      <c r="D8" s="3">
+        <v>0.35799999999999998</v>
       </c>
       <c r="E8">
         <v>0.19500000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
       </c>
       <c r="B9">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
       </c>
-      <c r="D9">
-        <v>0.35399999999999998</v>
+      <c r="D9" s="3">
+        <v>0.17599999999999999</v>
       </c>
       <c r="E9">
         <v>0.156</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2017</v>
-      </c>
-      <c r="C10" s="1" t="b">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>2016</v>
+      </c>
+      <c r="C10" t="b">
         <v>1</v>
       </c>
-      <c r="D10" s="1">
-        <v>0.41499999999999998</v>
+      <c r="D10" s="3">
+        <v>0.159</v>
       </c>
       <c r="E10" s="1">
         <v>0.30499999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
       </c>
-      <c r="D11">
-        <v>4.5999999999999999E-2</v>
+      <c r="D11" s="3">
+        <v>0.20499999999999999</v>
       </c>
       <c r="E11">
         <v>0.10100000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2018</v>
-      </c>
-      <c r="C12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2">
-        <v>9.1999999999999998E-2</v>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>2017</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.246</v>
       </c>
       <c r="E12">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>15</v>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
       </c>
-      <c r="D13">
-        <v>0.13100000000000001</v>
+      <c r="D13" s="3">
+        <v>0.104</v>
       </c>
       <c r="E13">
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>18</v>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>6</v>
       </c>
       <c r="B14">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
       </c>
-      <c r="D14">
-        <v>0.13100000000000001</v>
+      <c r="D14" s="3">
+        <v>0.30299999999999999</v>
       </c>
       <c r="E14">
         <v>0.185</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
       </c>
-      <c r="D15">
-        <v>0.23100000000000001</v>
+      <c r="D15" s="3">
+        <v>0.20899999999999999</v>
       </c>
       <c r="E15">
         <v>0.13300000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>16</v>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>8</v>
       </c>
       <c r="B16">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
       </c>
-      <c r="D16">
-        <v>0.23100000000000001</v>
+      <c r="D16" s="3">
+        <v>3.1E-2</v>
       </c>
       <c r="E16">
         <v>0.17699999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>17</v>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>9</v>
       </c>
       <c r="B17">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
       </c>
-      <c r="D17">
-        <v>0.32300000000000001</v>
+      <c r="D17" s="3">
+        <v>0.111</v>
       </c>
       <c r="E17" s="1">
         <v>0.218</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>14</v>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B18">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.48499999999999999</v>
+        <v>1</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.49099999999999999</v>
       </c>
       <c r="E18">
         <v>0.17199999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>20</v>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>11</v>
       </c>
       <c r="B19">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
       </c>
-      <c r="D19">
-        <v>8.5000000000000006E-2</v>
+      <c r="D19" s="3">
+        <v>0.29199999999999998</v>
       </c>
       <c r="E19">
         <v>8.1000000000000003E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>22</v>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>12</v>
       </c>
       <c r="B20">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0.108</v>
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.28000000000000003</v>
       </c>
       <c r="E20">
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>25</v>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>13</v>
       </c>
       <c r="B21">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
-      <c r="D21">
-        <v>0.115</v>
+      <c r="D21" s="3">
+        <v>0.32800000000000001</v>
       </c>
       <c r="E21">
         <v>0.16300000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>21</v>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>14</v>
       </c>
       <c r="B22">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
       </c>
-      <c r="D22">
-        <v>0.123</v>
+      <c r="D22" s="3">
+        <v>0.34499999999999997</v>
       </c>
       <c r="E22">
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>24</v>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>15</v>
       </c>
       <c r="B23">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
       </c>
-      <c r="D23">
-        <v>0.154</v>
+      <c r="D23" s="3">
+        <v>0.19800000000000001</v>
       </c>
       <c r="E23">
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>27</v>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>16</v>
       </c>
       <c r="B24">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
       </c>
-      <c r="D24">
-        <v>0.16900000000000001</v>
+      <c r="D24" s="3">
+        <v>0.28899999999999998</v>
       </c>
       <c r="E24">
         <v>0.14299999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>26</v>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B25">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
       </c>
-      <c r="D25">
-        <v>0.20799999999999999</v>
+      <c r="D25" s="4">
+        <v>0.39500000000000002</v>
       </c>
       <c r="E25">
         <v>0.105</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
-        <v>1917</v>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>18</v>
       </c>
       <c r="B26">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
       </c>
-      <c r="D26">
-        <v>0.308</v>
+      <c r="D26" s="3">
+        <v>0.254</v>
       </c>
       <c r="E26" s="1">
         <v>0.21099999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="1">
-        <v>2019</v>
-      </c>
-      <c r="C27" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0.438</v>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <v>2018</v>
+      </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>6.25E-2</v>
       </c>
       <c r="E27">
         <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1917</v>
+      </c>
+      <c r="B28">
+        <v>2019</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.38800000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>2019</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30">
+        <v>2019</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31">
+        <v>2019</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.20100000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32">
+        <v>2019</v>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.39400000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33">
+        <v>2019</v>
+      </c>
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.16900000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>2019</v>
+      </c>
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.30199999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35">
+        <v>2019</v>
+      </c>
+      <c r="C35" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36">
+        <v>2019</v>
+      </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>